<commit_message>
add user list to project
</commit_message>
<xml_diff>
--- a/output/2016-07-01 to 2016-08-01.xlsx
+++ b/output/2016-07-01 to 2016-08-01.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -74,10 +74,19 @@
     <t>project</t>
   </si>
   <si>
+    <t>users</t>
+  </si>
+  <si>
     <t>2016-06-103-01</t>
   </si>
   <si>
     <t>2016-08-101-01</t>
+  </si>
+  <si>
+    <t>['Shuchen Song']</t>
+  </si>
+  <si>
+    <t>['Hyung-Jin Yoon']</t>
   </si>
   <si>
     <t>cfop_MITRA</t>
@@ -652,13 +661,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
@@ -668,13 +677,16 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -682,19 +694,25 @@
       <c r="D2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3">
         <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -726,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -740,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>4</v>

</xml_diff>